<commit_message>
Fixed Chinese translation issue for month
Text was being fetched as UTF so wasn't working and wildcard for month wasn't set
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203773" uniqueCount="1910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213650" uniqueCount="1911">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6869,6 +6869,9 @@
   </si>
   <si>
     <t xml:space="preserve">Elapsed: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">月</t>
   </si>
 </sst>
 </file>
@@ -8396,7 +8399,9 @@
       <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="G13"/>
+      <c r="G13" t="s">
+        <v>1910</v>
+      </c>
       <c r="H13" t="s">
         <v>78</v>
       </c>
@@ -16846,6 +16851,9 @@
       <c r="G211" t="s">
         <v>43</v>
       </c>
+      <c r="H211" t="s">
+        <v>163</v>
+      </c>
       <c r="I211" t="s">
         <v>43</v>
       </c>

</xml_diff>